<commit_message>
Correcting names for outputs and obs data for soil mineral n
</commit_message>
<xml_diff>
--- a/Tests/Validation/Barley/Observations/MCPD09_10SoilNFinal.xlsx
+++ b/Tests/Validation/Barley/Observations/MCPD09_10SoilNFinal.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\ApsimX\Prototypes\Barley\Observations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Barley\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76678A7-001B-4CE9-8BF2-5E84BE0EEFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,31 +81,31 @@
     <t>MCPD09_10CultSherwoodNit150IrrNil</t>
   </si>
   <si>
-    <t>ProfileN</t>
-  </si>
-  <si>
-    <t>Soil.SoilNitrogen.mineral_n(1)</t>
-  </si>
-  <si>
-    <t>Soil.SoilNitrogen.mineral_n(2)</t>
-  </si>
-  <si>
-    <t>Soil.SoilNitrogen.mineral_n(3)</t>
-  </si>
-  <si>
-    <t>Soil.SoilNitrogen.mineral_n(4)</t>
-  </si>
-  <si>
-    <t>Soil.SoilNitrogen.mineral_n(5)</t>
-  </si>
-  <si>
-    <t>Soil.SoilNitrogen.mineral_n(6)</t>
+    <t>Soil.Nutrient.MineralN(1)</t>
+  </si>
+  <si>
+    <t>Soil.Nutrient.MineralN(2)</t>
+  </si>
+  <si>
+    <t>Soil.Nutrient.MineralN(3)</t>
+  </si>
+  <si>
+    <t>Soil.Nutrient.MineralN(4)</t>
+  </si>
+  <si>
+    <t>Soil.Nutrient.MineralN(5)</t>
+  </si>
+  <si>
+    <t>Soil.Nutrient.MineralN(6)</t>
+  </si>
+  <si>
+    <t>Soil.Nutrient.MineralN(7)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -419,20 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,28 +441,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -490,7 +491,7 @@
         <v>83.187139465121888</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -519,7 +520,7 @@
         <v>46.336136582874573</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -548,7 +549,7 @@
         <v>121.34756526090007</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -577,7 +578,7 @@
         <v>60.833504283874312</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -606,7 +607,7 @@
         <v>35.436549812865309</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -635,7 +636,7 @@
         <v>74.332627441331041</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -664,7 +665,7 @@
         <v>42.244512833787638</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -693,7 +694,7 @@
         <v>158.58928584210412</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -722,7 +723,7 @@
         <v>124.69507842874447</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -751,7 +752,7 @@
         <v>57.813414670018147</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -780,7 +781,7 @@
         <v>86.008286846387534</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -809,7 +810,7 @@
         <v>50.231568199923657</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -838,7 +839,7 @@
         <v>62.371307358099138</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -867,7 +868,7 @@
         <v>54.30532511395409</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -896,7 +897,7 @@
         <v>71.472179723092168</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>17</v>
       </c>

</xml_diff>